<commit_message>
Added Week 2 Day 5 materials
</commit_message>
<xml_diff>
--- a/Setup and Installation/Required Software and Setup.xlsx
+++ b/Setup and Installation/Required Software and Setup.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>Serial No.</t>
   </si>
@@ -156,6 +156,12 @@
     <t>https://jmeter.apache.org/download_jmeter.cgi</t>
   </si>
   <si>
+    <t>Firefox Browser</t>
+  </si>
+  <si>
+    <t>https://www.mozilla.org/en-US/firefox/new/</t>
+  </si>
+  <si>
     <t>Apache Tomcat  version 9</t>
   </si>
   <si>
@@ -185,10 +191,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -244,45 +250,83 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -299,74 +343,36 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -390,19 +396,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -414,163 +564,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -581,45 +587,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -634,9 +601,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -673,163 +642,200 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF7F7F7F"/>
       </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -853,7 +859,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="7" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="7" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1177,12 +1182,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A21" sqref="A21:C29"/>
+      <selection pane="bottomLeft" activeCell="A21" sqref="$A21:$XFD32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -1332,82 +1337,97 @@
       <c r="B19" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="C19" s="7" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" s="2"/>
     </row>
-    <row r="21" ht="17" customHeight="1" spans="1:3">
+    <row r="21" customFormat="1" ht="18.75" spans="1:3">
       <c r="A21" s="2">
         <v>10</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C21" s="10" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="23" ht="18.75" spans="1:4">
+    <row r="22" customFormat="1" ht="18.75" spans="2:3">
+      <c r="B22" s="6"/>
+      <c r="C22" s="10"/>
+    </row>
+    <row r="23" customFormat="1" ht="18.75" spans="1:3">
       <c r="A23" s="2">
         <v>11</v>
       </c>
-      <c r="B23" s="9" t="s">
+      <c r="B23" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="C23" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="D23" s="5"/>
-    </row>
-    <row r="24" spans="1:1">
+    </row>
+    <row r="24" customFormat="1" ht="18.75" spans="1:3">
       <c r="A24" s="2"/>
-    </row>
-    <row r="25" ht="18.75" spans="1:3">
+      <c r="B24" s="6"/>
+      <c r="C24" s="10"/>
+    </row>
+    <row r="25" customFormat="1" ht="17" customHeight="1" spans="1:3">
       <c r="A25" s="2">
         <v>12</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="3" t="s">
         <v>28</v>
       </c>
       <c r="C25" s="7" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:1">
+    <row r="26" customFormat="1" spans="1:1">
       <c r="A26" s="2"/>
     </row>
-    <row r="27" ht="18.75" spans="1:3">
+    <row r="27" customFormat="1" ht="18.75" spans="1:4">
       <c r="A27" s="2">
         <v>13</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C27" s="7" t="s">
+      <c r="C27" s="11" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="28" ht="18.75" spans="1:2">
-      <c r="A28" s="2"/>
-      <c r="B28" s="13"/>
-    </row>
-    <row r="29" spans="1:3">
+      <c r="D27" s="5"/>
+    </row>
+    <row r="28" customFormat="1"/>
+    <row r="29" customFormat="1" ht="18.75" spans="1:3">
       <c r="A29" s="2">
         <v>14</v>
       </c>
-      <c r="B29" t="s">
+      <c r="B29" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="7" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="30" ht="18.75" spans="1:2">
-      <c r="A30" s="2"/>
-      <c r="B30" s="13"/>
+    <row r="30" customFormat="1"/>
+    <row r="31" customFormat="1" ht="18.75" spans="1:3">
+      <c r="A31" s="2">
+        <v>15</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="32" customFormat="1" ht="18.75" spans="1:2">
+      <c r="A32" s="2"/>
+      <c r="B32" s="12"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1420,6 +1440,12 @@
     <hyperlink ref="C11" r:id="rId7" display="https://staruml.io/"/>
     <hyperlink ref="C17" r:id="rId8" display="https://dev.mysql.com/downloads/mysql/"/>
     <hyperlink ref="C19" r:id="rId9" display="https://www.mongodb.com/try/download/community"/>
+    <hyperlink ref="C31" r:id="rId10" display="https://nodejs.org/en/download/"/>
+    <hyperlink ref="C29" r:id="rId11" display="https://code.visualstudio.com/download"/>
+    <hyperlink ref="C27" r:id="rId12" display="https://www.postman.com/downloads/"/>
+    <hyperlink ref="C25" r:id="rId13" display="https://tomcat.apache.org/download-90.cgi"/>
+    <hyperlink ref="C21" r:id="rId14" display="https://jmeter.apache.org/download_jmeter.cgi"/>
+    <hyperlink ref="C23" r:id="rId15" display="https://www.mozilla.org/en-US/firefox/new/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Added Week 5 course materials
</commit_message>
<xml_diff>
--- a/Setup and Installation/Required Software and Setup.xlsx
+++ b/Setup and Installation/Required Software and Setup.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>Serial No.</t>
   </si>
@@ -185,16 +185,25 @@
   <si>
     <t>https://nodejs.org/en/download/</t>
   </si>
+  <si>
+    <t>Docker Desktop</t>
+  </si>
+  <si>
+    <t>https://www.docker.com/get-started/</t>
+  </si>
+  <si>
+    <t>Sign up for Docker Hub @ the same URL</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -251,31 +260,56 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -287,92 +321,67 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -396,13 +405,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -414,169 +585,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -599,13 +608,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -650,30 +663,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -687,18 +676,38 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
@@ -711,131 +720,131 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="18" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -860,9 +869,8 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="7" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="7"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1182,12 +1190,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="A21" sqref="$A21:$XFD32"/>
+      <selection pane="bottomLeft" activeCell="A33" sqref="$A33:$XFD33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -1401,7 +1409,6 @@
       </c>
       <c r="D27" s="5"/>
     </row>
-    <row r="28" customFormat="1"/>
     <row r="29" customFormat="1" ht="18.75" spans="1:3">
       <c r="A29" s="2">
         <v>14</v>
@@ -1413,7 +1420,6 @@
         <v>33</v>
       </c>
     </row>
-    <row r="30" customFormat="1"/>
     <row r="31" customFormat="1" ht="18.75" spans="1:3">
       <c r="A31" s="2">
         <v>15</v>
@@ -1427,7 +1433,21 @@
     </row>
     <row r="32" customFormat="1" ht="18.75" spans="1:2">
       <c r="A32" s="2"/>
-      <c r="B32" s="12"/>
+      <c r="B32" s="6"/>
+    </row>
+    <row r="33" ht="18.75" spans="1:4">
+      <c r="A33" s="2">
+        <v>16</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C33" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="D33" s="13" t="s">
+        <v>38</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1446,6 +1466,7 @@
     <hyperlink ref="C25" r:id="rId13" display="https://tomcat.apache.org/download-90.cgi"/>
     <hyperlink ref="C21" r:id="rId14" display="https://jmeter.apache.org/download_jmeter.cgi"/>
     <hyperlink ref="C23" r:id="rId15" display="https://www.mozilla.org/en-US/firefox/new/"/>
+    <hyperlink ref="C33" r:id="rId16" display="https://www.docker.com/get-started/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>